<commit_message>
Create Test Case for PHA Verification
</commit_message>
<xml_diff>
--- a/Test Patient Data.xlsx
+++ b/Test Patient Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\evils\Documents\UiPath\MedicalReadinessDiscrepancies\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A870B5C3-DDC1-4C36-97B1-8F6C2F8ED6AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB53DEB1-E226-4A76-B2D6-BFD1D9B9CAF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="19090" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="42">
   <si>
     <t>NMO NAME</t>
   </si>
@@ -109,6 +109,48 @@
   </si>
   <si>
     <t>MRRS Tet/Dipth Dt</t>
+  </si>
+  <si>
+    <t>PHA, CURRENT</t>
+  </si>
+  <si>
+    <t>xxx-xx-0001</t>
+  </si>
+  <si>
+    <t>-Annual Preventive Health Assessment is missing.:</t>
+  </si>
+  <si>
+    <t>OPOS</t>
+  </si>
+  <si>
+    <t>0001</t>
+  </si>
+  <si>
+    <t>Medical Immune</t>
+  </si>
+  <si>
+    <t>Negative</t>
+  </si>
+  <si>
+    <t>Normal</t>
+  </si>
+  <si>
+    <t>PHA, OVERDUE</t>
+  </si>
+  <si>
+    <t>xxx-xx-0002</t>
+  </si>
+  <si>
+    <t>0002</t>
+  </si>
+  <si>
+    <t>PHA, NONE</t>
+  </si>
+  <si>
+    <t>xxx-xx-0003</t>
+  </si>
+  <si>
+    <t>0003</t>
   </si>
 </sst>
 </file>
@@ -144,8 +186,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -426,19 +471,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AB1"/>
+  <dimension ref="A1:AB4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AB1" sqref="AB1"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.08984375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.36328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.7265625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.81640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.6328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="42.90625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.08984375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16.7265625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15.453125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="16.36328125" bestFit="1" customWidth="1"/>
@@ -461,7 +506,7 @@
     <col min="25" max="25" width="16.54296875" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="21.26953125" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="20.54296875" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="10.81640625" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:28" x14ac:dyDescent="0.35">
@@ -546,11 +591,270 @@
       <c r="AA1" t="s">
         <v>25</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AB1" s="3" t="s">
         <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" s="1">
+        <v>36526</v>
+      </c>
+      <c r="C2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F2" s="1">
+        <v>36526</v>
+      </c>
+      <c r="G2" t="s">
+        <v>31</v>
+      </c>
+      <c r="H2" s="1">
+        <v>45292</v>
+      </c>
+      <c r="I2" s="1">
+        <v>45293</v>
+      </c>
+      <c r="J2" s="1">
+        <v>45294</v>
+      </c>
+      <c r="K2" t="s">
+        <v>35</v>
+      </c>
+      <c r="L2" s="1">
+        <v>45295</v>
+      </c>
+      <c r="M2" t="s">
+        <v>34</v>
+      </c>
+      <c r="N2" s="1">
+        <v>45296</v>
+      </c>
+      <c r="O2" s="1">
+        <v>45297</v>
+      </c>
+      <c r="P2" s="1">
+        <v>45298</v>
+      </c>
+      <c r="Q2" s="1">
+        <v>45299</v>
+      </c>
+      <c r="R2" t="s">
+        <v>33</v>
+      </c>
+      <c r="S2" s="1">
+        <v>45300</v>
+      </c>
+      <c r="T2" t="s">
+        <v>33</v>
+      </c>
+      <c r="U2" s="1">
+        <v>45301</v>
+      </c>
+      <c r="V2" s="1">
+        <v>45302</v>
+      </c>
+      <c r="W2" t="s">
+        <v>33</v>
+      </c>
+      <c r="X2" s="1">
+        <v>45303</v>
+      </c>
+      <c r="Y2" s="1">
+        <v>45304</v>
+      </c>
+      <c r="Z2" s="1">
+        <v>45305</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>33</v>
+      </c>
+      <c r="AB2" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B3" s="1">
+        <v>36526</v>
+      </c>
+      <c r="C3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E3" t="s">
+        <v>36</v>
+      </c>
+      <c r="F3" s="1">
+        <v>36526</v>
+      </c>
+      <c r="G3" t="s">
+        <v>31</v>
+      </c>
+      <c r="H3" s="1">
+        <v>45292</v>
+      </c>
+      <c r="I3" s="1">
+        <v>45293</v>
+      </c>
+      <c r="J3" s="1">
+        <v>45294</v>
+      </c>
+      <c r="K3" t="s">
+        <v>35</v>
+      </c>
+      <c r="L3" s="1">
+        <v>45295</v>
+      </c>
+      <c r="M3" t="s">
+        <v>34</v>
+      </c>
+      <c r="N3" s="1">
+        <v>36526</v>
+      </c>
+      <c r="O3" s="1">
+        <v>45297</v>
+      </c>
+      <c r="P3" s="1">
+        <v>45298</v>
+      </c>
+      <c r="Q3" s="1">
+        <v>45299</v>
+      </c>
+      <c r="R3" t="s">
+        <v>33</v>
+      </c>
+      <c r="S3" s="1">
+        <v>45300</v>
+      </c>
+      <c r="T3" t="s">
+        <v>33</v>
+      </c>
+      <c r="U3" s="1">
+        <v>45301</v>
+      </c>
+      <c r="V3" s="1">
+        <v>45302</v>
+      </c>
+      <c r="W3" t="s">
+        <v>33</v>
+      </c>
+      <c r="X3" s="1">
+        <v>45303</v>
+      </c>
+      <c r="Y3" s="1">
+        <v>45304</v>
+      </c>
+      <c r="Z3" s="1">
+        <v>45305</v>
+      </c>
+      <c r="AA3" t="s">
+        <v>33</v>
+      </c>
+      <c r="AB3" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="4" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B4" s="1">
+        <v>36526</v>
+      </c>
+      <c r="C4" t="s">
+        <v>40</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E4" t="s">
+        <v>39</v>
+      </c>
+      <c r="F4" s="1">
+        <v>36526</v>
+      </c>
+      <c r="G4" t="s">
+        <v>31</v>
+      </c>
+      <c r="H4" s="1">
+        <v>45292</v>
+      </c>
+      <c r="I4" s="1">
+        <v>45293</v>
+      </c>
+      <c r="J4" s="1">
+        <v>45294</v>
+      </c>
+      <c r="K4" t="s">
+        <v>35</v>
+      </c>
+      <c r="L4" s="1">
+        <v>45295</v>
+      </c>
+      <c r="M4" t="s">
+        <v>34</v>
+      </c>
+      <c r="N4" s="1"/>
+      <c r="O4" s="1">
+        <v>45297</v>
+      </c>
+      <c r="P4" s="1">
+        <v>45298</v>
+      </c>
+      <c r="Q4" s="1">
+        <v>45299</v>
+      </c>
+      <c r="R4" t="s">
+        <v>33</v>
+      </c>
+      <c r="S4" s="1">
+        <v>45300</v>
+      </c>
+      <c r="T4" t="s">
+        <v>33</v>
+      </c>
+      <c r="U4" s="1">
+        <v>45301</v>
+      </c>
+      <c r="V4" s="1">
+        <v>45302</v>
+      </c>
+      <c r="W4" t="s">
+        <v>33</v>
+      </c>
+      <c r="X4" s="1">
+        <v>45303</v>
+      </c>
+      <c r="Y4" s="1">
+        <v>45304</v>
+      </c>
+      <c r="Z4" s="1">
+        <v>45305</v>
+      </c>
+      <c r="AA4" t="s">
+        <v>33</v>
+      </c>
+      <c r="AB4" s="3" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <ignoredErrors>
+    <ignoredError sqref="AB2" numberStoredAsText="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Create Test Case for PHA Updated in MRRS
</commit_message>
<xml_diff>
--- a/Test Patient Data.xlsx
+++ b/Test Patient Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\evils\Documents\UiPath\MedicalReadinessDiscrepancies\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB53DEB1-E226-4A76-B2D6-BFD1D9B9CAF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD4C3697-9F14-4C6F-AECC-D4DCF171E1B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="19090" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="58">
   <si>
     <t>NMO NAME</t>
   </si>
@@ -151,16 +151,70 @@
   </si>
   <si>
     <t>0003</t>
+  </si>
+  <si>
+    <t>01-Jan-2000</t>
+  </si>
+  <si>
+    <t>02-Jan-2000</t>
+  </si>
+  <si>
+    <t>03-Jan-2000</t>
+  </si>
+  <si>
+    <t>04-Jan-2000</t>
+  </si>
+  <si>
+    <t>05-Jan-2000</t>
+  </si>
+  <si>
+    <t>01-Jan-2024</t>
+  </si>
+  <si>
+    <t>07-Jan-2000</t>
+  </si>
+  <si>
+    <t>08-Jan-2000</t>
+  </si>
+  <si>
+    <t>09-Jan-2000</t>
+  </si>
+  <si>
+    <t>10-Jan-2000</t>
+  </si>
+  <si>
+    <t>11-Jan-2000</t>
+  </si>
+  <si>
+    <t>12-Jan-2000</t>
+  </si>
+  <si>
+    <t>13-Jan-2000</t>
+  </si>
+  <si>
+    <t>14-Jan-2000</t>
+  </si>
+  <si>
+    <t>15-Jan-2000</t>
+  </si>
+  <si>
+    <t>06-Jan-2000</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -474,7 +528,7 @@
   <dimension ref="A1:AB4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -484,27 +538,27 @@
     <col min="3" max="3" width="10.6328125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="42.90625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.08984375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.7265625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.7265625" style="3" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15.453125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.36328125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.7265625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="17.08984375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.36328125" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.7265625" style="3" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.08984375" style="3" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="17.1796875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="20.54296875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="20.54296875" style="3" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="20.6328125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11.90625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="15.36328125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="17.08984375" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="18.7265625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.90625" style="3" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15.36328125" style="3" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="17.08984375" style="3" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="18.7265625" style="3" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="18.08984375" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="18.6328125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="18.6328125" style="3" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="18" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="16.26953125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="18.7265625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="16.26953125" style="3" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="18.7265625" style="3" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="18.08984375" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="12.54296875" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="16.54296875" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="21.26953125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="12.54296875" style="3" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="16.54296875" style="3" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="21.26953125" style="3" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="20.54296875" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="10.81640625" style="3" bestFit="1" customWidth="1"/>
   </cols>
@@ -525,67 +579,67 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
       <c r="G1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="3" t="s">
         <v>9</v>
       </c>
       <c r="K1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="L1" s="3" t="s">
         <v>11</v>
       </c>
       <c r="M1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="s">
+      <c r="N1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="O1" t="s">
+      <c r="O1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="P1" t="s">
+      <c r="P1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="Q1" s="3" t="s">
         <v>16</v>
       </c>
       <c r="R1" t="s">
         <v>17</v>
       </c>
-      <c r="S1" t="s">
+      <c r="S1" s="3" t="s">
         <v>18</v>
       </c>
       <c r="T1" t="s">
         <v>19</v>
       </c>
-      <c r="U1" t="s">
+      <c r="U1" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="V1" t="s">
+      <c r="V1" s="3" t="s">
         <v>21</v>
       </c>
       <c r="W1" t="s">
         <v>22</v>
       </c>
-      <c r="X1" t="s">
+      <c r="X1" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Y1" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="Z1" s="3" t="s">
         <v>24</v>
       </c>
       <c r="AA1" t="s">
@@ -611,68 +665,68 @@
       <c r="E2" t="s">
         <v>28</v>
       </c>
-      <c r="F2" s="1">
-        <v>36526</v>
+      <c r="F2" s="3" t="s">
+        <v>42</v>
       </c>
       <c r="G2" t="s">
         <v>31</v>
       </c>
-      <c r="H2" s="1">
-        <v>45292</v>
-      </c>
-      <c r="I2" s="1">
-        <v>45293</v>
-      </c>
-      <c r="J2" s="1">
-        <v>45294</v>
+      <c r="H2" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>45</v>
       </c>
       <c r="K2" t="s">
         <v>35</v>
       </c>
-      <c r="L2" s="1">
-        <v>45295</v>
+      <c r="L2" s="3" t="s">
+        <v>46</v>
       </c>
       <c r="M2" t="s">
         <v>34</v>
       </c>
-      <c r="N2" s="1">
-        <v>45296</v>
-      </c>
-      <c r="O2" s="1">
-        <v>45297</v>
-      </c>
-      <c r="P2" s="1">
-        <v>45298</v>
-      </c>
-      <c r="Q2" s="1">
-        <v>45299</v>
+      <c r="N2" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="O2" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="P2" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q2" s="3" t="s">
+        <v>50</v>
       </c>
       <c r="R2" t="s">
         <v>33</v>
       </c>
-      <c r="S2" s="1">
-        <v>45300</v>
+      <c r="S2" s="3" t="s">
+        <v>51</v>
       </c>
       <c r="T2" t="s">
         <v>33</v>
       </c>
-      <c r="U2" s="1">
-        <v>45301</v>
-      </c>
-      <c r="V2" s="1">
-        <v>45302</v>
+      <c r="U2" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="V2" s="3" t="s">
+        <v>53</v>
       </c>
       <c r="W2" t="s">
         <v>33</v>
       </c>
-      <c r="X2" s="1">
-        <v>45303</v>
-      </c>
-      <c r="Y2" s="1">
-        <v>45304</v>
-      </c>
-      <c r="Z2" s="1">
-        <v>45305</v>
+      <c r="X2" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="Y2" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="Z2" s="3" t="s">
+        <v>56</v>
       </c>
       <c r="AA2" t="s">
         <v>33</v>
@@ -697,68 +751,68 @@
       <c r="E3" t="s">
         <v>36</v>
       </c>
-      <c r="F3" s="1">
-        <v>36526</v>
+      <c r="F3" s="3" t="s">
+        <v>42</v>
       </c>
       <c r="G3" t="s">
         <v>31</v>
       </c>
-      <c r="H3" s="1">
-        <v>45292</v>
-      </c>
-      <c r="I3" s="1">
-        <v>45293</v>
-      </c>
-      <c r="J3" s="1">
-        <v>45294</v>
+      <c r="H3" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>45</v>
       </c>
       <c r="K3" t="s">
         <v>35</v>
       </c>
-      <c r="L3" s="1">
-        <v>45295</v>
+      <c r="L3" s="3" t="s">
+        <v>46</v>
       </c>
       <c r="M3" t="s">
         <v>34</v>
       </c>
-      <c r="N3" s="1">
-        <v>36526</v>
-      </c>
-      <c r="O3" s="1">
-        <v>45297</v>
-      </c>
-      <c r="P3" s="1">
-        <v>45298</v>
-      </c>
-      <c r="Q3" s="1">
-        <v>45299</v>
+      <c r="N3" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="O3" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="P3" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q3" s="3" t="s">
+        <v>50</v>
       </c>
       <c r="R3" t="s">
         <v>33</v>
       </c>
-      <c r="S3" s="1">
-        <v>45300</v>
+      <c r="S3" s="3" t="s">
+        <v>51</v>
       </c>
       <c r="T3" t="s">
         <v>33</v>
       </c>
-      <c r="U3" s="1">
-        <v>45301</v>
-      </c>
-      <c r="V3" s="1">
-        <v>45302</v>
+      <c r="U3" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="V3" s="3" t="s">
+        <v>53</v>
       </c>
       <c r="W3" t="s">
         <v>33</v>
       </c>
-      <c r="X3" s="1">
-        <v>45303</v>
-      </c>
-      <c r="Y3" s="1">
-        <v>45304</v>
-      </c>
-      <c r="Z3" s="1">
-        <v>45305</v>
+      <c r="X3" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="Y3" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="Z3" s="3" t="s">
+        <v>56</v>
       </c>
       <c r="AA3" t="s">
         <v>33</v>
@@ -783,66 +837,65 @@
       <c r="E4" t="s">
         <v>39</v>
       </c>
-      <c r="F4" s="1">
-        <v>36526</v>
+      <c r="F4" s="3" t="s">
+        <v>42</v>
       </c>
       <c r="G4" t="s">
         <v>31</v>
       </c>
-      <c r="H4" s="1">
-        <v>45292</v>
-      </c>
-      <c r="I4" s="1">
-        <v>45293</v>
-      </c>
-      <c r="J4" s="1">
-        <v>45294</v>
+      <c r="H4" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>45</v>
       </c>
       <c r="K4" t="s">
         <v>35</v>
       </c>
-      <c r="L4" s="1">
-        <v>45295</v>
+      <c r="L4" s="3" t="s">
+        <v>46</v>
       </c>
       <c r="M4" t="s">
         <v>34</v>
       </c>
-      <c r="N4" s="1"/>
-      <c r="O4" s="1">
-        <v>45297</v>
-      </c>
-      <c r="P4" s="1">
-        <v>45298</v>
-      </c>
-      <c r="Q4" s="1">
-        <v>45299</v>
+      <c r="O4" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="P4" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q4" s="3" t="s">
+        <v>50</v>
       </c>
       <c r="R4" t="s">
         <v>33</v>
       </c>
-      <c r="S4" s="1">
-        <v>45300</v>
+      <c r="S4" s="3" t="s">
+        <v>51</v>
       </c>
       <c r="T4" t="s">
         <v>33</v>
       </c>
-      <c r="U4" s="1">
-        <v>45301</v>
-      </c>
-      <c r="V4" s="1">
-        <v>45302</v>
+      <c r="U4" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="V4" s="3" t="s">
+        <v>53</v>
       </c>
       <c r="W4" t="s">
         <v>33</v>
       </c>
-      <c r="X4" s="1">
-        <v>45303</v>
-      </c>
-      <c r="Y4" s="1">
-        <v>45304</v>
-      </c>
-      <c r="Z4" s="1">
-        <v>45305</v>
+      <c r="X4" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="Y4" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="Z4" s="3" t="s">
+        <v>56</v>
       </c>
       <c r="AA4" t="s">
         <v>33</v>
@@ -852,6 +905,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
     <ignoredError sqref="AB2" numberStoredAsText="1"/>

</xml_diff>

<commit_message>
Add logic for determining test case success (or failure)
</commit_message>
<xml_diff>
--- a/Test Patient Data.xlsx
+++ b/Test Patient Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\evils\Documents\UiPath\MedicalReadinessDiscrepancies\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D066B84C-631A-4E47-9D1D-C3F0A26B22F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{464D8A4E-89FC-4368-A296-21431E4D3357}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19090" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PHA" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="37">
   <si>
     <t>NMO NAME</t>
   </si>
@@ -606,7 +606,7 @@
   <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -745,6 +745,9 @@
       <c r="C5" t="s">
         <v>29</v>
       </c>
+      <c r="D5" s="1" t="s">
+        <v>22</v>
+      </c>
       <c r="E5" t="s">
         <v>28</v>
       </c>

</xml_diff>

<commit_message>
Add checks for TDAP delinquency in MRRS
</commit_message>
<xml_diff>
--- a/Test Patient Data.xlsx
+++ b/Test Patient Data.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\evils\Documents\UiPath\MedicalReadinessDiscrepancies\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{464D8A4E-89FC-4368-A296-21431E4D3357}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C525A425-B695-4595-B85D-A58D25A3ACB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19090" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19090" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PHA" sheetId="1" r:id="rId1"/>
     <sheet name="HIV" sheetId="2" r:id="rId2"/>
+    <sheet name="TDAP" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="42">
   <si>
     <t>NMO NAME</t>
   </si>
@@ -148,6 +149,21 @@
   </si>
   <si>
     <t>HIV, NONE</t>
+  </si>
+  <si>
+    <t>-TD Vaccination is missing.:</t>
+  </si>
+  <si>
+    <t>TDAP, CURRENT</t>
+  </si>
+  <si>
+    <t>TDAP, OVERDUE</t>
+  </si>
+  <si>
+    <t>TDAP, NONE</t>
+  </si>
+  <si>
+    <t>MRRS Tet/Dipth Dt</t>
   </si>
 </sst>
 </file>
@@ -605,7 +621,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79844CF7-75DC-4D62-90BB-F5B7624EC2EE}">
   <dimension ref="A1:I5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
@@ -762,4 +778,130 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{487A2340-C829-44E4-B724-BE7C1E5B0908}">
+  <dimension ref="A1:H4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="14.08984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.36328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.6328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="42.90625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.08984375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.7265625" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.54296875" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.81640625" style="2" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E3" t="s">
+        <v>39</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E4" t="s">
+        <v>40</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Add logic to check for Polio vaccination date
</commit_message>
<xml_diff>
--- a/Test Patient Data.xlsx
+++ b/Test Patient Data.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\evils\Documents\UiPath\MedicalReadinessDiscrepancies\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C525A425-B695-4595-B85D-A58D25A3ACB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAC7149F-E947-4AD4-B8B6-C22552A8DF3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19090" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19090" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PHA" sheetId="1" r:id="rId1"/>
     <sheet name="HIV" sheetId="2" r:id="rId2"/>
     <sheet name="TDAP" sheetId="4" r:id="rId3"/>
+    <sheet name="Polio" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="46">
   <si>
     <t>NMO NAME</t>
   </si>
@@ -164,6 +165,18 @@
   </si>
   <si>
     <t>MRRS Tet/Dipth Dt</t>
+  </si>
+  <si>
+    <t>-POLIO Vaccination is missing.:</t>
+  </si>
+  <si>
+    <t>POLIO, CURRENT</t>
+  </si>
+  <si>
+    <t>POLIO, NONE</t>
+  </si>
+  <si>
+    <t>MRRS Polio Dt</t>
   </si>
 </sst>
 </file>
@@ -784,8 +797,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{487A2340-C829-44E4-B724-BE7C1E5B0908}">
   <dimension ref="A1:H4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2:H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -904,4 +917,104 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F62AB438-AC2C-4942-83C0-84D06B33E8BA}">
+  <dimension ref="A1:H3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="14.36328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.6328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.36328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.08984375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.7265625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.54296875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.81640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E2" t="s">
+        <v>43</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" t="s">
+        <v>42</v>
+      </c>
+      <c r="E3" t="s">
+        <v>44</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Initial commit (Flu verification test case)
</commit_message>
<xml_diff>
--- a/Test Patient Data.xlsx
+++ b/Test Patient Data.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\evils\Documents\UiPath\MedicalReadinessDiscrepancies\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAC7149F-E947-4AD4-B8B6-C22552A8DF3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5916FA68-C180-4612-9284-DE152522E0B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19090" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19090" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PHA" sheetId="1" r:id="rId1"/>
     <sheet name="HIV" sheetId="2" r:id="rId2"/>
     <sheet name="TDAP" sheetId="4" r:id="rId3"/>
     <sheet name="Polio" sheetId="5" r:id="rId4"/>
+    <sheet name="Influenza" sheetId="7" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="59">
   <si>
     <t>NMO NAME</t>
   </si>
@@ -177,6 +178,45 @@
   </si>
   <si>
     <t>MRRS Polio Dt</t>
+  </si>
+  <si>
+    <t>-FLU shot is due.:</t>
+  </si>
+  <si>
+    <t>FLU, CURRENT POSTSEP</t>
+  </si>
+  <si>
+    <t>FLU, CURRENT PRESEP</t>
+  </si>
+  <si>
+    <t>MRRS Influenza Dt</t>
+  </si>
+  <si>
+    <t>FLU, NONE</t>
+  </si>
+  <si>
+    <t>-FLU Vaccination is missing.:</t>
+  </si>
+  <si>
+    <t>xxx-xx-0005</t>
+  </si>
+  <si>
+    <t>0005</t>
+  </si>
+  <si>
+    <t>Current Date</t>
+  </si>
+  <si>
+    <t>30-Sep-2024</t>
+  </si>
+  <si>
+    <t>FLU, OVERDUE POSTSEP</t>
+  </si>
+  <si>
+    <t>FLU, OVERDUE PRESEP</t>
+  </si>
+  <si>
+    <t>30-Sep-2023</t>
   </si>
 </sst>
 </file>
@@ -218,10 +258,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -923,7 +964,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F62AB438-AC2C-4942-83C0-84D06B33E8BA}">
   <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
@@ -1017,4 +1058,201 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{041EEB8E-71A9-4B1B-A351-2646D6EF0F13}">
+  <dimension ref="A1:I6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I4" sqref="I4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="23.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.6328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.36328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.36328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.7265625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.26953125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.54296875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2" t="s">
+        <v>47</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="I2" s="3">
+        <v>45627</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" t="s">
+        <v>46</v>
+      </c>
+      <c r="E3" t="s">
+        <v>48</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I3" s="3">
+        <v>45688</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>56</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" t="s">
+        <v>46</v>
+      </c>
+      <c r="E4" t="s">
+        <v>47</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I4" s="3">
+        <v>45627</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>57</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D5" t="s">
+        <v>46</v>
+      </c>
+      <c r="E5" t="s">
+        <v>48</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="I5" s="3">
+        <v>45688</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>50</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" t="s">
+        <v>52</v>
+      </c>
+      <c r="D6" t="s">
+        <v>51</v>
+      </c>
+      <c r="E6" t="s">
+        <v>50</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="I6" s="3">
+        <v>45627</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Update test data so current date is in correct format
</commit_message>
<xml_diff>
--- a/Test Patient Data.xlsx
+++ b/Test Patient Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\evils\Documents\UiPath\MedicalReadinessDiscrepancies\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5916FA68-C180-4612-9284-DE152522E0B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9ACC5F22-851E-4DD0-8BE7-887A1618AA31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="19090" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="61">
   <si>
     <t>NMO NAME</t>
   </si>
@@ -217,6 +217,12 @@
   </si>
   <si>
     <t>30-Sep-2023</t>
+  </si>
+  <si>
+    <t>01-Dec-2024</t>
+  </si>
+  <si>
+    <t>31-Jan-2025</t>
   </si>
 </sst>
 </file>
@@ -258,11 +264,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1062,10 +1067,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{041EEB8E-71A9-4B1B-A351-2646D6EF0F13}">
-  <dimension ref="A1:I6"/>
+  <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1077,7 +1082,8 @@
     <col min="6" max="6" width="16.7265625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="16.26953125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10.81640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.54296875" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.1796875" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.35">
@@ -1134,8 +1140,8 @@
       <c r="H2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I2" s="3">
-        <v>45627</v>
+      <c r="I2" s="2" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
@@ -1163,8 +1169,8 @@
       <c r="H3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="I3" s="3">
-        <v>45688</v>
+      <c r="I3" s="2" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.35">
@@ -1192,8 +1198,8 @@
       <c r="H4" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="I4" s="3">
-        <v>45627</v>
+      <c r="I4" s="2" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.35">
@@ -1221,8 +1227,8 @@
       <c r="H5" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="I5" s="3">
-        <v>45688</v>
+      <c r="I5" s="2" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.35">
@@ -1247,12 +1253,13 @@
       <c r="H6" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="I6" s="3">
-        <v>45627</v>
+      <c r="I6" s="2" t="s">
+        <v>59</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Create test case template for blood type testing
</commit_message>
<xml_diff>
--- a/Test Patient Data.xlsx
+++ b/Test Patient Data.xlsx
@@ -8,16 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\evils\Documents\UiPath\MedicalReadinessDiscrepancies\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9ACC5F22-851E-4DD0-8BE7-887A1618AA31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E0A5816-D378-4AB7-9452-EB0AC3E23E9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19090" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19090" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PHA" sheetId="1" r:id="rId1"/>
     <sheet name="HIV" sheetId="2" r:id="rId2"/>
-    <sheet name="TDAP" sheetId="4" r:id="rId3"/>
-    <sheet name="Polio" sheetId="5" r:id="rId4"/>
-    <sheet name="Influenza" sheetId="7" r:id="rId5"/>
+    <sheet name="Blood Type" sheetId="8" r:id="rId3"/>
+    <sheet name="TDAP" sheetId="4" r:id="rId4"/>
+    <sheet name="Polio" sheetId="5" r:id="rId5"/>
+    <sheet name="Influenza" sheetId="7" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="69">
   <si>
     <t>NMO NAME</t>
   </si>
@@ -223,6 +224,30 @@
   </si>
   <si>
     <t>31-Jan-2025</t>
+  </si>
+  <si>
+    <t>-Blood Type Data is missing.:</t>
+  </si>
+  <si>
+    <t>BLOOD TYPE, CURRENT</t>
+  </si>
+  <si>
+    <t>BLOOD TYPE, MISSING TYPE</t>
+  </si>
+  <si>
+    <t>BLOOD TYPE, MISSING ALL</t>
+  </si>
+  <si>
+    <t>MRRS G6PD Test Dt</t>
+  </si>
+  <si>
+    <t>30-Sep-2020</t>
+  </si>
+  <si>
+    <t>MRRS Blood Type</t>
+  </si>
+  <si>
+    <t>OPOS</t>
   </si>
 </sst>
 </file>
@@ -840,6 +865,186 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46B62407-4A7A-433A-BC5E-BD13617799CC}">
+  <dimension ref="A1:K5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="23.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.6328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.36328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.7265625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.7265625" customWidth="1"/>
+    <col min="8" max="8" width="17.08984375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.54296875" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.1796875" style="2" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" t="s">
+        <v>61</v>
+      </c>
+      <c r="E2" t="s">
+        <v>62</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>63</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" t="s">
+        <v>61</v>
+      </c>
+      <c r="E3" t="s">
+        <v>63</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>63</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" t="s">
+        <v>61</v>
+      </c>
+      <c r="E4" t="s">
+        <v>63</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>64</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D5" t="s">
+        <v>61</v>
+      </c>
+      <c r="E5" t="s">
+        <v>64</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{487A2340-C829-44E4-B724-BE7C1E5B0908}">
   <dimension ref="A1:H4"/>
   <sheetViews>
@@ -965,7 +1170,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F62AB438-AC2C-4942-83C0-84D06B33E8BA}">
   <dimension ref="A1:H3"/>
   <sheetViews>
@@ -1065,11 +1270,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{041EEB8E-71A9-4B1B-A351-2646D6EF0F13}">
   <dimension ref="A1:J6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Fixed test data (two rows had the same patient name)
</commit_message>
<xml_diff>
--- a/Test Patient Data.xlsx
+++ b/Test Patient Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\evils\Documents\UiPath\MedicalReadinessDiscrepancies\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E0A5816-D378-4AB7-9452-EB0AC3E23E9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E5F225C-6850-4F42-A894-BB3BCA3BE2B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="19090" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="70">
   <si>
     <t>NMO NAME</t>
   </si>
@@ -248,6 +248,9 @@
   </si>
   <si>
     <t>OPOS</t>
+  </si>
+  <si>
+    <t>BLOOD TYPE, MISSING DATE</t>
   </si>
 </sst>
 </file>
@@ -869,7 +872,7 @@
   <dimension ref="A1:K5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -982,7 +985,7 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>21</v>
@@ -994,7 +997,7 @@
         <v>61</v>
       </c>
       <c r="E4" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>18</v>

</xml_diff>